<commit_message>
EPBDS-8299 Fix 'transform to' return type. Add tests
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_orderBy.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_orderBy.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="27795" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="27795" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mode &amp; Methodsl" sheetId="3" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
+    <sheet name="Rules" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="147">
   <si>
     <t>String</t>
   </si>
@@ -366,19 +367,113 @@
   </si>
   <si>
     <t>#W</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult calc(Integer i)</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>= i</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>= i / 3</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult case1(Integer[] i)</t>
+  </si>
+  <si>
+    <t>SumS</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>SumF</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>= calc(i)</t>
+  </si>
+  <si>
+    <t>= sum ($Calc$B($Calc))</t>
+  </si>
+  <si>
+    <t>= flatten ($Calc$B($Calc))</t>
+  </si>
+  <si>
+    <t>= sum ($Flat)</t>
+  </si>
+  <si>
+    <t>= $SumS == $SumF</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>= $A == $B</t>
+  </si>
+  <si>
+    <t>=allTrue($A, $B, $SumS, $SumF)</t>
+  </si>
+  <si>
+    <t>Test case1</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>_res_.$E$Q</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>= $A[ order by $Calc$A ]</t>
+  </si>
+  <si>
+    <t>3,1,2,3,2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -413,20 +508,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -767,10 +870,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -789,11 +892,11 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
       <c r="F9" s="1" t="s">
         <v>91</v>
       </c>
@@ -950,7 +1053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AG42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
@@ -989,42 +1092,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="U2" s="4" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="U2" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
     </row>
     <row r="3" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -2008,42 +2111,42 @@
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="F23" s="4" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="F23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="U23" s="4" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="U23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
-      <c r="AC23" s="4"/>
-      <c r="AD23" s="4"/>
-      <c r="AE23" s="4"/>
-      <c r="AF23" s="4"/>
-      <c r="AG23" s="4"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7"/>
+      <c r="AC23" s="7"/>
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
@@ -3034,4 +3137,202 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" style="4" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13" style="4" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="4" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-13025 The empty array elements are trimmed
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_orderBy.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Arrays_orderBy.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF4DDADD-2EBC-4F6B-82D9-6E587BC4DE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="27795" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="16760" yWindow="2950" windowWidth="19930" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode &amp; Methodsl" sheetId="3" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="146">
   <si>
     <t>String</t>
   </si>
@@ -304,9 +310,6 @@
   </si>
   <si>
     <t>1,3,8,10,5,9</t>
-  </si>
-  <si>
-    <t>,</t>
   </si>
   <si>
     <t>9,5,1,10,8,3</t>
@@ -462,7 +465,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -512,11 +515,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -528,8 +529,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -556,7 +557,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -565,14 +566,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -610,9 +614,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,9 +649,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -680,9 +701,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -855,27 +893,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +921,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -891,17 +929,17 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="F9" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
@@ -915,7 +953,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -926,7 +964,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -940,7 +978,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -954,7 +992,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>3</v>
       </c>
@@ -965,7 +1003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>4</v>
       </c>
@@ -976,7 +1014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>5</v>
       </c>
@@ -987,7 +1025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
         <v>6</v>
       </c>
@@ -998,7 +1036,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <v>7</v>
       </c>
@@ -1009,7 +1047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <v>8</v>
       </c>
@@ -1020,7 +1058,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <v>9</v>
       </c>
@@ -1031,7 +1069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <v>10</v>
       </c>
@@ -1050,86 +1088,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AG42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:AG41"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="U2" s="7" t="s">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="U2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-    </row>
-    <row r="3" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+    </row>
+    <row r="3" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
@@ -1185,22 +1223,22 @@
         <v>32</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>73</v>
@@ -1221,7 +1259,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -1261,7 +1299,7 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1314,7 +1352,7 @@
         <v>85</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>2</v>
@@ -1345,7 +1383,7 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1390,7 +1428,7 @@
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="U6" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1409,7 +1447,7 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1454,7 +1492,7 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="U7" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V7" s="1" t="s">
         <v>2</v>
@@ -1477,7 +1515,7 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1526,7 +1564,7 @@
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="U8" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>3</v>
@@ -1549,7 +1587,7 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
@@ -1598,7 +1636,7 @@
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="U9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
@@ -1613,7 +1651,7 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1652,7 +1690,7 @@
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1660,7 +1698,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>50</v>
@@ -1691,7 +1729,7 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
@@ -1742,12 +1780,12 @@
       </c>
       <c r="S12" s="1"/>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>30</v>
@@ -1756,7 +1794,7 @@
         <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>19</v>
@@ -1793,20 +1831,16 @@
       </c>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="F14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1820,7 +1854,7 @@
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1861,7 +1895,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
@@ -1894,7 +1928,7 @@
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>60</v>
       </c>
@@ -1947,7 +1981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
@@ -2000,7 +2034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
@@ -2051,7 +2085,7 @@
       </c>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>69</v>
       </c>
@@ -2102,53 +2136,45 @@
       </c>
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.35">
+      <c r="B23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="F23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="U23" s="7" t="s">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="U23" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
-      <c r="AA23" s="7"/>
-      <c r="AB23" s="7"/>
-      <c r="AC23" s="7"/>
-      <c r="AD23" s="7"/>
-      <c r="AE23" s="7"/>
-      <c r="AF23" s="7"/>
-      <c r="AG23" s="7"/>
-    </row>
-    <row r="24" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
+    </row>
+    <row r="24" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
@@ -2204,22 +2230,22 @@
         <v>32</v>
       </c>
       <c r="V24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="W24" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="W24" s="1" t="s">
+      <c r="X24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA24" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y24" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="Z24" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA24" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="AB24" s="1" t="s">
         <v>73</v>
@@ -2240,7 +2266,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>8</v>
@@ -2280,7 +2306,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row r="26" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>44</v>
       </c>
@@ -2333,7 +2359,7 @@
         <v>85</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V26" s="1" t="s">
         <v>2</v>
@@ -2364,7 +2390,7 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
     </row>
-    <row r="27" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
         <v>33</v>
       </c>
@@ -2409,7 +2435,7 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="U27" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
@@ -2428,7 +2454,7 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
     </row>
-    <row r="28" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>34</v>
       </c>
@@ -2473,7 +2499,7 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="U28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="V28" s="1" t="s">
         <v>2</v>
@@ -2496,7 +2522,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row r="29" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
@@ -2504,7 +2530,7 @@
         <v>22</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>47</v>
@@ -2545,7 +2571,7 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="U29" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="V29" s="1" t="s">
         <v>3</v>
@@ -2568,7 +2594,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row r="30" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2576,7 +2602,7 @@
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>48</v>
@@ -2617,7 +2643,7 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="U30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
@@ -2632,7 +2658,7 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
@@ -2671,7 +2697,7 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
     </row>
-    <row r="32" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>38</v>
       </c>
@@ -2679,7 +2705,7 @@
         <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>50</v>
@@ -2710,7 +2736,7 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
@@ -2718,7 +2744,7 @@
         <v>95</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>51</v>
@@ -2761,21 +2787,21 @@
       </c>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>52</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>15</v>
@@ -2812,20 +2838,16 @@
       </c>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="F35" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>96</v>
-      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -2839,7 +2861,7 @@
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>42</v>
       </c>
@@ -2880,7 +2902,7 @@
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>43</v>
       </c>
@@ -2913,7 +2935,7 @@
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>60</v>
       </c>
@@ -2921,7 +2943,7 @@
         <v>58</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>56</v>
@@ -2966,7 +2988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
         <v>61</v>
       </c>
@@ -2974,7 +2996,7 @@
         <v>59</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>57</v>
@@ -3019,7 +3041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>68</v>
       </c>
@@ -3070,7 +3092,7 @@
       </c>
       <c r="S40" s="1"/>
     </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>69</v>
       </c>
@@ -3078,7 +3100,7 @@
         <v>67</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>65</v>
@@ -3120,10 +3142,6 @@
         <v>20</v>
       </c>
       <c r="S41" s="1"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3140,189 +3158,189 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="40.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.28515625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13" style="4" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="4" collapsed="1"/>
+    <col min="1" max="1" width="2.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.26953125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.26953125" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.81640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.1796875" style="2" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="5" t="s">
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="5" t="s">
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="E8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G9" s="5" t="s">
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C16" s="5" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="5" t="s">
+      <c r="C17" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>142</v>
+      <c r="C18" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>